<commit_message>
restructuring of files and attempting asynchronous again
</commit_message>
<xml_diff>
--- a/old/all_results_after_excl.xlsx
+++ b/old/all_results_after_excl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlh\Desktop\PycharmProjects\Bayes_Opt\old\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449584E3-A4F2-4AFD-8456-5184EE87E963}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBF0B40-DBF8-41DD-8D26-E4C86BCDDD9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Avg and stdev" sheetId="7" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="all_results" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -6420,8 +6421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7241,8 +7242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView topLeftCell="E5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28150,7 +28151,7 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <f t="shared" ref="E23:X23" si="0">IF(E2=E22, 1, 0)</f>
+        <f t="shared" ref="E23:W23" si="0">IF(E2=E22, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="F23">

</xml_diff>